<commit_message>
Add interpretation to the line graph
</commit_message>
<xml_diff>
--- a/Proposal's Data Sets/Concentration_of_Carbon_dioxide_1959_to_2020.xlsx
+++ b/Proposal's Data Sets/Concentration_of_Carbon_dioxide_1959_to_2020.xlsx
@@ -850,11 +850,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>